<commit_message>
Update on LED scenario for services sector
Energy service demand requirements have been updated for LED scenario
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SYS_Demands_LED_highlighted.xlsx
+++ b/SuppXLS/Scen_SYS_Demands_LED_highlighted.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rbsul\Documents\GitHub\times-ireland-model-VAv2\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8885AB85-763D-47A2-A5A8-9997EF5456D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89FF6C1C-C870-46EC-8E8F-0F2DB82B1633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2805" yWindow="1815" windowWidth="19200" windowHeight="11175" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BY-Demands" sheetId="5" r:id="rId1"/>
@@ -1002,9 +1002,6 @@
     <t>deact~TFM_Fill-R: w=Inputs_RSD; Hcol=Region</t>
   </si>
   <si>
-    <t>~TFM_Fill-R: w=Inputs_SRV; Hcol=Region</t>
-  </si>
-  <si>
     <t>S-BLD_CS</t>
   </si>
   <si>
@@ -1012,6 +1009,9 @@
   </si>
   <si>
     <t>%</t>
+  </si>
+  <si>
+    <t>deact~TFM_Fill-R: w=Inputs_SRV; Hcol=Region</t>
   </si>
 </sst>
 </file>
@@ -9389,7 +9389,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C1:AQ90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
@@ -24723,7 +24723,7 @@
   <dimension ref="C7:V22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R9" sqref="R9:R22"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24745,7 +24745,7 @@
       <c r="J7" s="36"/>
       <c r="K7" s="36"/>
       <c r="N7" s="41" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="O7" s="35"/>
       <c r="P7" s="35"/>
@@ -25322,8 +25322,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2523A896-A3FC-4F9A-B5DF-A205D08521A3}">
   <dimension ref="C3:O33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25394,7 +25394,7 @@
       <c r="K5" s="28"/>
       <c r="L5" s="28"/>
       <c r="N5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="O5">
         <v>2018</v>
@@ -25405,10 +25405,11 @@
         <v>151</v>
       </c>
       <c r="F6">
-        <v>2025</v>
+        <v>2022</v>
       </c>
       <c r="G6">
-        <v>0.29750119328038643</v>
+        <f>O6</f>
+        <v>0.30754680541104201</v>
       </c>
       <c r="I6" t="s">
         <v>163</v>
@@ -25418,7 +25419,7 @@
       </c>
       <c r="N6" s="49">
         <f>+G6/O6*100%</f>
-        <v>0.96733631449291291</v>
+        <v>1</v>
       </c>
       <c r="O6">
         <f>+SUMIF(Inputs_SRV!$D$2:$D$15,Services!I6,Inputs_SRV!$L$2:$L$15)</f>
@@ -25430,10 +25431,11 @@
         <v>151</v>
       </c>
       <c r="F7">
-        <v>2025</v>
+        <v>2022</v>
       </c>
       <c r="G7">
-        <v>7.8240205489280165E-2</v>
+        <f t="shared" ref="G7:G19" si="0">O7</f>
+        <v>8.6436286608257501E-2</v>
       </c>
       <c r="I7" t="s">
         <v>164</v>
@@ -25442,8 +25444,8 @@
         <v>164</v>
       </c>
       <c r="N7" s="49">
-        <f t="shared" ref="N7:N19" si="0">+G7/O7*100%</f>
-        <v>0.90517777381942344</v>
+        <f t="shared" ref="N7:N19" si="1">+G7/O7*100%</f>
+        <v>1</v>
       </c>
       <c r="O7">
         <f>+SUMIF(Inputs_SRV!$D$2:$D$15,Services!I7,Inputs_SRV!$L$2:$L$15)</f>
@@ -25455,10 +25457,11 @@
         <v>151</v>
       </c>
       <c r="F8">
-        <v>2025</v>
+        <v>2022</v>
       </c>
       <c r="G8">
-        <v>9.9230285582155173E-2</v>
+        <f t="shared" si="0"/>
+        <v>0.125158654758175</v>
       </c>
       <c r="I8" t="s">
         <v>165</v>
@@ -25467,8 +25470,8 @@
         <v>165</v>
       </c>
       <c r="N8" s="49">
-        <f t="shared" si="0"/>
-        <v>0.79283598704286762</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="O8">
         <f>+SUMIF(Inputs_SRV!$D$2:$D$15,Services!I8,Inputs_SRV!$L$2:$L$15)</f>
@@ -25480,10 +25483,11 @@
         <v>151</v>
       </c>
       <c r="F9">
-        <v>2025</v>
+        <v>2022</v>
       </c>
       <c r="G9">
-        <v>0.1299964335480952</v>
+        <f t="shared" si="0"/>
+        <v>0.135247613114969</v>
       </c>
       <c r="I9" t="s">
         <v>166</v>
@@ -25492,8 +25496,8 @@
         <v>166</v>
       </c>
       <c r="N9" s="49">
-        <f t="shared" si="0"/>
-        <v>0.96117358786650109</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="O9">
         <f>+SUMIF(Inputs_SRV!$D$2:$D$15,Services!I9,Inputs_SRV!$L$2:$L$15)</f>
@@ -25505,9 +25509,10 @@
         <v>151</v>
       </c>
       <c r="F10">
-        <v>2025</v>
+        <v>2022</v>
       </c>
       <c r="G10">
+        <f t="shared" si="0"/>
         <v>0.65611067742996398</v>
       </c>
       <c r="I10" t="s">
@@ -25517,7 +25522,7 @@
         <v>167</v>
       </c>
       <c r="N10" s="49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="O10">
@@ -25530,10 +25535,11 @@
         <v>151</v>
       </c>
       <c r="F11">
-        <v>2025</v>
+        <v>2022</v>
       </c>
       <c r="G11">
-        <v>3.4112422198348336</v>
+        <f t="shared" si="0"/>
+        <v>3.41124221983483</v>
       </c>
       <c r="I11" t="s">
         <v>168</v>
@@ -25542,8 +25548,8 @@
         <v>168</v>
       </c>
       <c r="N11" s="49">
-        <f t="shared" si="0"/>
-        <v>1.0000000000000011</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="O11">
         <f>+SUMIF(Inputs_SRV!$D$2:$D$15,Services!I11,Inputs_SRV!$L$2:$L$15)</f>
@@ -25555,10 +25561,11 @@
         <v>151</v>
       </c>
       <c r="F12">
-        <v>2025</v>
+        <v>2022</v>
       </c>
       <c r="G12">
-        <v>0.27048899641521007</v>
+        <f t="shared" si="0"/>
+        <v>0.34149098112577198</v>
       </c>
       <c r="I12" t="s">
         <v>169</v>
@@ -25567,8 +25574,8 @@
         <v>169</v>
       </c>
       <c r="N12" s="49">
-        <f t="shared" si="0"/>
-        <v>0.79208240148394515</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="O12">
         <f>+SUMIF(Inputs_SRV!$D$2:$D$15,Services!I12,Inputs_SRV!$L$2:$L$15)</f>
@@ -25580,10 +25587,11 @@
         <v>151</v>
       </c>
       <c r="F13">
-        <v>2025</v>
+        <v>2022</v>
       </c>
       <c r="G13">
-        <v>0.14436837706846065</v>
+        <f t="shared" si="0"/>
+        <v>0.104177979439828</v>
       </c>
       <c r="I13" t="s">
         <v>170</v>
@@ -25592,8 +25600,8 @@
         <v>170</v>
       </c>
       <c r="N13" s="49">
-        <f t="shared" si="0"/>
-        <v>1.3857859198723101</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="O13">
         <f>+SUMIF(Inputs_SRV!$D$2:$D$15,Services!I13,Inputs_SRV!$L$2:$L$15)</f>
@@ -25605,10 +25613,11 @@
         <v>151</v>
       </c>
       <c r="F14">
-        <v>2025</v>
+        <v>2022</v>
       </c>
       <c r="G14">
-        <v>3.5851150535518087E-2</v>
+        <f t="shared" si="0"/>
+        <v>2.5794975305082499E-2</v>
       </c>
       <c r="I14" t="s">
         <v>171</v>
@@ -25617,8 +25626,8 @@
         <v>171</v>
       </c>
       <c r="N14" s="49">
-        <f t="shared" si="0"/>
-        <v>1.3898501592460983</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="O14">
         <f>+SUMIF(Inputs_SRV!$D$2:$D$15,Services!I14,Inputs_SRV!$L$2:$L$15)</f>
@@ -25630,10 +25639,11 @@
         <v>151</v>
       </c>
       <c r="F15">
-        <v>2025</v>
+        <v>2022</v>
       </c>
       <c r="G15">
-        <v>2.7014519280249845E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.93475483290594E-2</v>
       </c>
       <c r="I15" t="s">
         <v>172</v>
@@ -25642,8 +25652,8 @@
         <v>172</v>
       </c>
       <c r="N15" s="49">
-        <f t="shared" si="0"/>
-        <v>1.396276097663232</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="O15">
         <f>+SUMIF(Inputs_SRV!$D$2:$D$15,Services!I15,Inputs_SRV!$L$2:$L$15)</f>
@@ -25655,10 +25665,11 @@
         <v>151</v>
       </c>
       <c r="F16">
-        <v>2025</v>
+        <v>2022</v>
       </c>
       <c r="G16">
-        <v>3.8223383014175182E-2</v>
+        <f t="shared" si="0"/>
+        <v>3.2190254153783002E-2</v>
       </c>
       <c r="I16" t="s">
         <v>173</v>
@@ -25667,8 +25678,8 @@
         <v>173</v>
       </c>
       <c r="N16" s="49">
-        <f t="shared" si="0"/>
-        <v>1.1874209762858665</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="O16">
         <f>+SUMIF(Inputs_SRV!$D$2:$D$15,Services!I16,Inputs_SRV!$L$2:$L$15)</f>
@@ -25680,10 +25691,11 @@
         <v>151</v>
       </c>
       <c r="F17">
-        <v>2025</v>
+        <v>2022</v>
       </c>
       <c r="G17">
-        <v>0.16206914757843674</v>
+        <f t="shared" si="0"/>
+        <v>0.16206914757843699</v>
       </c>
       <c r="I17" t="s">
         <v>174</v>
@@ -25692,8 +25704,8 @@
         <v>174</v>
       </c>
       <c r="N17" s="49">
-        <f t="shared" si="0"/>
-        <v>0.99999999999999845</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="O17">
         <f>+SUMIF(Inputs_SRV!$D$2:$D$15,Services!I17,Inputs_SRV!$L$2:$L$15)</f>
@@ -25705,10 +25717,11 @@
         <v>151</v>
       </c>
       <c r="F18">
-        <v>2025</v>
+        <v>2022</v>
       </c>
       <c r="G18">
-        <v>0.84262783364201532</v>
+        <f t="shared" si="0"/>
+        <v>0.84262783364201499</v>
       </c>
       <c r="I18" t="s">
         <v>175</v>
@@ -25717,8 +25730,8 @@
         <v>175</v>
       </c>
       <c r="N18" s="49">
-        <f t="shared" si="0"/>
-        <v>1.0000000000000004</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="O18">
         <f>+SUMIF(Inputs_SRV!$D$2:$D$15,Services!I18,Inputs_SRV!$L$2:$L$15)</f>
@@ -25730,10 +25743,11 @@
         <v>151</v>
       </c>
       <c r="F19">
-        <v>2025</v>
+        <v>2022</v>
       </c>
       <c r="G19">
-        <v>7.3395482092335179E-2</v>
+        <f t="shared" si="0"/>
+        <v>5.2612374241425702E-2</v>
       </c>
       <c r="I19" t="s">
         <v>176</v>
@@ -25742,8 +25756,8 @@
         <v>176</v>
       </c>
       <c r="N19" s="49">
-        <f t="shared" si="0"/>
-        <v>1.3950231889467812</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="O19">
         <f>+SUMIF(Inputs_SRV!$D$2:$D$15,Services!I19,Inputs_SRV!$L$2:$L$15)</f>
@@ -25758,7 +25772,8 @@
         <v>2050</v>
       </c>
       <c r="G20">
-        <v>0.16362565630421255</v>
+        <f>+G6*(1-N20)</f>
+        <v>0.16915074297607313</v>
       </c>
       <c r="I20" t="s">
         <v>163</v>
@@ -25767,8 +25782,7 @@
         <v>163</v>
       </c>
       <c r="N20" s="49">
-        <f>+G20/G6</f>
-        <v>0.55000000000000004</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="21" spans="5:15" x14ac:dyDescent="0.25">
@@ -25779,7 +25793,8 @@
         <v>2050</v>
       </c>
       <c r="G21">
-        <v>4.3032113019104097E-2</v>
+        <f t="shared" ref="G21:G33" si="2">+G7*(1-N21)</f>
+        <v>4.7539957634541628E-2</v>
       </c>
       <c r="I21" t="s">
         <v>164</v>
@@ -25788,8 +25803,7 @@
         <v>164</v>
       </c>
       <c r="N21" s="49">
-        <f t="shared" ref="N21:N33" si="1">+G21/G7</f>
-        <v>0.55000000000000004</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="22" spans="5:15" x14ac:dyDescent="0.25">
@@ -25800,7 +25814,8 @@
         <v>2050</v>
       </c>
       <c r="G22">
-        <v>5.4576657070185351E-2</v>
+        <f t="shared" si="2"/>
+        <v>6.8837260116996257E-2</v>
       </c>
       <c r="I22" t="s">
         <v>165</v>
@@ -25809,8 +25824,7 @@
         <v>165</v>
       </c>
       <c r="N22" s="49">
-        <f t="shared" si="1"/>
-        <v>0.55000000000000004</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="23" spans="5:15" x14ac:dyDescent="0.25">
@@ -25821,7 +25835,8 @@
         <v>2050</v>
       </c>
       <c r="G23">
-        <v>7.1498038451452361E-2</v>
+        <f t="shared" si="2"/>
+        <v>7.4386187213232952E-2</v>
       </c>
       <c r="I23" t="s">
         <v>166</v>
@@ -25830,8 +25845,7 @@
         <v>166</v>
       </c>
       <c r="N23" s="49">
-        <f t="shared" si="1"/>
-        <v>0.55000000000000004</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="24" spans="5:15" x14ac:dyDescent="0.25">
@@ -25842,6 +25856,7 @@
         <v>2050</v>
       </c>
       <c r="G24">
+        <f t="shared" si="2"/>
         <v>0.3608608725864802</v>
       </c>
       <c r="I24" t="s">
@@ -25851,8 +25866,7 @@
         <v>167</v>
       </c>
       <c r="N24" s="49">
-        <f t="shared" si="1"/>
-        <v>0.55000000000000004</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="25" spans="5:15" x14ac:dyDescent="0.25">
@@ -25863,7 +25877,8 @@
         <v>2050</v>
       </c>
       <c r="G25">
-        <v>1.8761832209091587</v>
+        <f t="shared" si="2"/>
+        <v>1.8761832209091567</v>
       </c>
       <c r="I25" t="s">
         <v>168</v>
@@ -25872,8 +25887,7 @@
         <v>168</v>
       </c>
       <c r="N25" s="49">
-        <f t="shared" si="1"/>
-        <v>0.55000000000000004</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="26" spans="5:15" x14ac:dyDescent="0.25">
@@ -25884,7 +25898,8 @@
         <v>2050</v>
       </c>
       <c r="G26">
-        <v>0.14876894802836554</v>
+        <f t="shared" si="2"/>
+        <v>0.18782003961917459</v>
       </c>
       <c r="I26" t="s">
         <v>169</v>
@@ -25893,8 +25908,7 @@
         <v>169</v>
       </c>
       <c r="N26" s="49">
-        <f t="shared" si="1"/>
-        <v>0.55000000000000004</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="27" spans="5:15" x14ac:dyDescent="0.25">
@@ -25905,7 +25919,8 @@
         <v>2050</v>
       </c>
       <c r="G27">
-        <v>7.9402607387653368E-2</v>
+        <f t="shared" si="2"/>
+        <v>5.7297888691905406E-2</v>
       </c>
       <c r="I27" t="s">
         <v>170</v>
@@ -25914,8 +25929,7 @@
         <v>170</v>
       </c>
       <c r="N27" s="49">
-        <f t="shared" si="1"/>
-        <v>0.55000000000000004</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="28" spans="5:15" x14ac:dyDescent="0.25">
@@ -25926,7 +25940,8 @@
         <v>2050</v>
       </c>
       <c r="G28">
-        <v>1.9718132794534948E-2</v>
+        <f t="shared" si="2"/>
+        <v>1.4187236417795375E-2</v>
       </c>
       <c r="I28" t="s">
         <v>171</v>
@@ -25935,8 +25950,7 @@
         <v>171</v>
       </c>
       <c r="N28" s="49">
-        <f t="shared" si="1"/>
-        <v>0.55000000000000004</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="29" spans="5:15" x14ac:dyDescent="0.25">
@@ -25947,7 +25961,8 @@
         <v>2050</v>
       </c>
       <c r="G29">
-        <v>1.4857985604137416E-2</v>
+        <f t="shared" si="2"/>
+        <v>1.0641151580982671E-2</v>
       </c>
       <c r="I29" t="s">
         <v>172</v>
@@ -25956,8 +25971,7 @@
         <v>172</v>
       </c>
       <c r="N29" s="49">
-        <f t="shared" si="1"/>
-        <v>0.55000000000000004</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="30" spans="5:15" x14ac:dyDescent="0.25">
@@ -25968,7 +25982,8 @@
         <v>2050</v>
       </c>
       <c r="G30">
-        <v>2.1022860657796353E-2</v>
+        <f t="shared" si="2"/>
+        <v>1.7704639784580652E-2</v>
       </c>
       <c r="I30" t="s">
         <v>173</v>
@@ -25977,8 +25992,7 @@
         <v>173</v>
       </c>
       <c r="N30" s="49">
-        <f t="shared" si="1"/>
-        <v>0.55000000000000004</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="31" spans="5:15" x14ac:dyDescent="0.25">
@@ -25989,7 +26003,8 @@
         <v>2050</v>
       </c>
       <c r="G31">
-        <v>8.9138031168140217E-2</v>
+        <f t="shared" si="2"/>
+        <v>8.9138031168140355E-2</v>
       </c>
       <c r="I31" t="s">
         <v>174</v>
@@ -25998,8 +26013,7 @@
         <v>174</v>
       </c>
       <c r="N31" s="49">
-        <f t="shared" si="1"/>
-        <v>0.55000000000000004</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="32" spans="5:15" x14ac:dyDescent="0.25">
@@ -26010,7 +26024,8 @@
         <v>2050</v>
       </c>
       <c r="G32">
-        <v>0.46344530850310844</v>
+        <f t="shared" si="2"/>
+        <v>0.46344530850310828</v>
       </c>
       <c r="I32" t="s">
         <v>175</v>
@@ -26019,8 +26034,7 @@
         <v>175</v>
       </c>
       <c r="N32" s="49">
-        <f t="shared" si="1"/>
-        <v>0.55000000000000004</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="33" spans="5:14" x14ac:dyDescent="0.25">
@@ -26031,7 +26045,8 @@
         <v>2050</v>
       </c>
       <c r="G33">
-        <v>4.036751515078435E-2</v>
+        <f t="shared" si="2"/>
+        <v>2.893680583278414E-2</v>
       </c>
       <c r="I33" t="s">
         <v>176</v>
@@ -26040,8 +26055,7 @@
         <v>176</v>
       </c>
       <c r="N33" s="49">
-        <f t="shared" si="1"/>
-        <v>0.55000000000000004</v>
+        <v>0.45</v>
       </c>
     </row>
   </sheetData>
@@ -26112,7 +26126,7 @@
         <v>151</v>
       </c>
       <c r="C2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D2" t="s">
         <v>166</v>
@@ -26153,7 +26167,7 @@
         <v>151</v>
       </c>
       <c r="C3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D3" t="s">
         <v>167</v>
@@ -26194,7 +26208,7 @@
         <v>151</v>
       </c>
       <c r="C4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D4" t="s">
         <v>169</v>
@@ -26235,7 +26249,7 @@
         <v>151</v>
       </c>
       <c r="C5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D5" t="s">
         <v>168</v>
@@ -26276,7 +26290,7 @@
         <v>151</v>
       </c>
       <c r="C6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D6" t="s">
         <v>165</v>
@@ -26317,7 +26331,7 @@
         <v>151</v>
       </c>
       <c r="C7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D7" t="s">
         <v>163</v>
@@ -26358,7 +26372,7 @@
         <v>151</v>
       </c>
       <c r="C8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D8" t="s">
         <v>164</v>
@@ -26399,7 +26413,7 @@
         <v>151</v>
       </c>
       <c r="C9" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D9" t="s">
         <v>173</v>
@@ -26440,7 +26454,7 @@
         <v>151</v>
       </c>
       <c r="C10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D10" t="s">
         <v>174</v>
@@ -26481,7 +26495,7 @@
         <v>151</v>
       </c>
       <c r="C11" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D11" t="s">
         <v>176</v>
@@ -26522,7 +26536,7 @@
         <v>151</v>
       </c>
       <c r="C12" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D12" t="s">
         <v>175</v>
@@ -26563,7 +26577,7 @@
         <v>151</v>
       </c>
       <c r="C13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D13" t="s">
         <v>172</v>
@@ -26604,7 +26618,7 @@
         <v>151</v>
       </c>
       <c r="C14" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D14" t="s">
         <v>170</v>
@@ -26645,7 +26659,7 @@
         <v>151</v>
       </c>
       <c r="C15" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D15" t="s">
         <v>171</v>

</xml_diff>